<commit_message>
Added another problem to discuss
</commit_message>
<xml_diff>
--- a/30.04.17/Problems&Solutions.xlsx
+++ b/30.04.17/Problems&Solutions.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Problem</t>
   </si>
@@ -62,6 +62,9 @@
   </si>
   <si>
     <t>6. twitter reliability or twitter's reliability</t>
+  </si>
+  <si>
+    <t>7. Do we need to number abbreviations as reference numbers</t>
   </si>
 </sst>
 </file>
@@ -414,10 +417,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -490,6 +493,11 @@
         <v>15</v>
       </c>
     </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
updated the styles of excel sheet
</commit_message>
<xml_diff>
--- a/30.04.17/Problems&Solutions.xlsx
+++ b/30.04.17/Problems&Solutions.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -79,7 +79,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -215,23 +215,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -267,23 +250,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -462,7 +428,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -470,6 +436,7 @@
   <cols>
     <col min="1" max="1" width="118.85546875" customWidth="1"/>
     <col min="2" max="3" width="52.5703125" customWidth="1"/>
+    <col min="4" max="4" width="63.5703125" customWidth="1"/>
     <col min="6" max="6" width="11.5703125" customWidth="1"/>
     <col min="10" max="10" width="12.28515625" customWidth="1"/>
   </cols>

</xml_diff>